<commit_message>
add new test for control null values
</commit_message>
<xml_diff>
--- a/src/test/resources/calculations.xlsx
+++ b/src/test/resources/calculations.xlsx
@@ -1,51 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lionita\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Explanatory note" sheetId="2" r:id="rId1"/>
-    <sheet name="SI calculations" sheetId="1" r:id="rId2"/>
+    <sheet name="Explanatory note" sheetId="1" r:id="rId4"/>
+    <sheet name="SI calculations" sheetId="2" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Explanatory note'!$B$1:$P$11</definedName>
-  </definedNames>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
-    <t>ISIN</t>
+    <t>Systematic internaliser calculations - Results File</t>
   </si>
   <si>
-    <t>Total number of transactions executed in the EU</t>
+    <t>Explanations</t>
   </si>
   <si>
-    <t>Systematic internaliser calculations - Results File</t>
+    <t>The results are published only for instruments for which trading venues submitted data for at least 95% of all trading days over the 6-month observation period.</t>
+  </si>
+  <si>
+    <t>The fields "Calculation From Date" and "Calculation To Date" refer to the reference period of the data considered to perform the EU aggregation.</t>
+  </si>
+  <si>
+    <t>The value of the "Total turnover executed in the EU" is expressed in euros.</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>Explanations</t>
-  </si>
-  <si>
-    <t>The value of the "Total turnover executed in the EU" is expressed in euros.</t>
+    <t>This file has been published on DD MMM YYYY.</t>
   </si>
   <si>
     <t>Calculation From Date</t>
@@ -54,16 +41,13 @@
     <t>Calculation To Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Total turnover executed in the EU </t>
+    <t>ISIN</t>
   </si>
   <si>
-    <t>The fields "Calculation From Date" and "Calculation To Date" refer to the reference period of the data considered to perform the EU aggregation.</t>
+    <t>Total number of transactions executed in the EU</t>
   </si>
   <si>
-    <t>The results are published only for instruments for which trading venues submitted data for at least 95% of all trading days over the 6-month observation period.</t>
-  </si>
-  <si>
-    <t>This file has been published on DD MMM YYYY.</t>
+    <t xml:space="preserve">Total turnover executed in the EU </t>
   </si>
   <si>
     <t>ABXXXXXXXXXX</t>
@@ -81,61 +65,48 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="&quot; &quot;* #,##0.00&quot; &quot;;&quot;-&quot;* #,##0.00&quot; &quot;;&quot; &quot;* &quot;-&quot;??&quot; &quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="10"/>
+      <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
-      <color theme="0"/>
+      <color indexed="9"/>
       <name val="Arial"/>
-      <family val="2"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -147,18 +118,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF2D4190"/>
-        <bgColor indexed="64"/>
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor indexed="11"/>
+        <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="15">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -168,116 +188,253 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
+      <right style="thin">
+        <color indexed="10"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color indexed="10"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color indexed="8"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="25">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="59" fontId="3" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 12 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0"/>
   <colors>
-    <mruColors>
-      <color rgb="FF0000FF"/>
-    </mruColors>
+    <indexedColors>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff2d4190"/>
+    </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2209800" cy="904875"/>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2082800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="esma_8_V3"/>
-        <xdr:cNvPicPr/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
+        <a:blip r:embed="rId1">
+          <a:extLst/>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
           <a:off x="114300" y="120650"/>
           <a:ext cx="2209800" cy="904875"/>
@@ -285,29 +442,33 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office Theme">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="5B9BD5"/>
@@ -328,85 +489,25 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="FF00FF"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office Theme">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office Theme">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -415,76 +516,66 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
+                <a:tint val="100000"/>
                 <a:shade val="100000"/>
+                <a:satMod val="129999"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="104999"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -495,129 +586,992 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </a:spPr>
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+        <a:spAutoFit/>
+      </a:bodyPr>
+      <a:lstStyle>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
+          </a:defRPr>
+        </a:defPPr>
+        <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl1pPr>
+        <a:lvl2pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl2pPr>
+        <a:lvl3pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl3pPr>
+        <a:lvl4pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl4pPr>
+        <a:lvl5pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl5pPr>
+        <a:lvl6pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl6pPr>
+        <a:lvl7pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl7pPr>
+        <a:lvl8pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl8pPr>
+        <a:lvl9pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl9pPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="none"/>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </a:spPr>
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+        <a:noAutofit/>
+      </a:bodyPr>
+      <a:lstStyle>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:defPPr>
+        <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl1pPr>
+        <a:lvl2pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl2pPr>
+        <a:lvl3pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl3pPr>
+        <a:lvl4pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl4pPr>
+        <a:lvl5pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl5pPr>
+        <a:lvl6pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl6pPr>
+        <a:lvl7pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl7pPr>
+        <a:lvl8pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl8pPr>
+        <a:lvl9pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl9pPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="none"/>
+      </a:style>
+    </a:lnDef>
+    <a:txDef>
+      <a:spPr>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </a:spPr>
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+        <a:spAutoFit/>
+      </a:bodyPr>
+      <a:lstStyle>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
+          </a:defRPr>
+        </a:defPPr>
+        <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl1pPr>
+        <a:lvl2pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl2pPr>
+        <a:lvl3pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl3pPr>
+        <a:lvl4pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl4pPr>
+        <a:lvl5pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl5pPr>
+        <a:lvl6pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl6pPr>
+        <a:lvl7pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl7pPr>
+        <a:lvl8pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl8pPr>
+        <a:lvl9pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+          </a:defRPr>
+        </a:lvl9pPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="none"/>
+      </a:style>
+    </a:txDef>
+  </a:objectDefaults>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AK51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.16667" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="164.5703125" style="5" customWidth="1"/>
-    <col min="3" max="10" width="9.140625" style="5"/>
-    <col min="11" max="11" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="9.140625" style="5"/>
-    <col min="15" max="15" width="30.5703125" style="5" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="5" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="3.17188" style="1" customWidth="1"/>
+    <col min="2" max="2" width="164.5" style="1" customWidth="1"/>
+    <col min="3" max="10" width="9.17188" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6719" style="1" customWidth="1"/>
+    <col min="12" max="14" width="9.17188" style="1" customWidth="1"/>
+    <col min="15" max="15" width="30.5" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.17188" style="1" customWidth="1"/>
+    <col min="17" max="17" width="2.67188" style="1" customWidth="1"/>
+    <col min="18" max="37" width="9.17188" style="1" customWidth="1"/>
+    <col min="38" max="256" width="9.17188" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="4"/>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -653,9 +1607,10 @@
       <c r="AH2" s="6"/>
       <c r="AI2" s="6"/>
       <c r="AJ2" s="6"/>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="AK2" s="4"/>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -691,9 +1646,10 @@
       <c r="AH3" s="6"/>
       <c r="AI3" s="6"/>
       <c r="AJ3" s="6"/>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="AK3" s="4"/>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -729,9 +1685,10 @@
       <c r="AH4" s="6"/>
       <c r="AI4" s="6"/>
       <c r="AJ4" s="6"/>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="AK4" s="4"/>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -767,9 +1724,10 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="6"/>
       <c r="AJ5" s="6"/>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="AK5" s="4"/>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -805,9 +1763,10 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="6"/>
       <c r="AJ6" s="6"/>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="AK6" s="4"/>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -843,113 +1802,114 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="6"/>
       <c r="AJ7" s="6"/>
-    </row>
-    <row r="8" spans="1:37" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="10" t="s">
-        <v>2</v>
+      <c r="AK7" s="7"/>
+    </row>
+    <row r="8" ht="34.5" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" t="s" s="8">
+        <v>0</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="8"/>
-      <c r="AI8" s="8"/>
-      <c r="AJ8" s="8"/>
-      <c r="AK8" s="8"/>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="9"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" s="5"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="8"/>
-      <c r="AB9" s="8"/>
-      <c r="AC9" s="8"/>
-      <c r="AD9" s="8"/>
-      <c r="AE9" s="8"/>
-      <c r="AF9" s="8"/>
-      <c r="AG9" s="8"/>
-      <c r="AH9" s="8"/>
-      <c r="AI9" s="8"/>
-      <c r="AJ9" s="8"/>
-      <c r="AK9" s="8"/>
-    </row>
-    <row r="10" spans="1:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="9" t="s">
-        <v>4</v>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
+      <c r="AJ9" s="6"/>
+      <c r="AK9" s="9"/>
+    </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" t="s" s="10">
+        <v>1</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
@@ -963,31 +1923,32 @@
       <c r="AH10" s="6"/>
       <c r="AI10" s="6"/>
       <c r="AJ10" s="6"/>
-    </row>
-    <row r="11" spans="1:37" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
+      <c r="AK10" s="11"/>
+    </row>
+    <row r="11" ht="8" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
       <c r="X11" s="6"/>
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
@@ -1001,11 +1962,12 @@
       <c r="AH11" s="6"/>
       <c r="AI11" s="6"/>
       <c r="AJ11" s="6"/>
-    </row>
-    <row r="12" spans="1:37" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="11" t="s">
-        <v>10</v>
+      <c r="AK11" s="4"/>
+    </row>
+    <row r="12" ht="33.75" customHeight="1">
+      <c r="A12" s="5"/>
+      <c r="B12" t="s" s="12">
+        <v>2</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -1041,11 +2003,12 @@
       <c r="AH12" s="6"/>
       <c r="AI12" s="6"/>
       <c r="AJ12" s="6"/>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7" t="s">
-        <v>9</v>
+      <c r="AK12" s="4"/>
+    </row>
+    <row r="13" ht="15" customHeight="1">
+      <c r="A13" s="5"/>
+      <c r="B13" t="s" s="13">
+        <v>3</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -1081,11 +2044,12 @@
       <c r="AH13" s="6"/>
       <c r="AI13" s="6"/>
       <c r="AJ13" s="6"/>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7" t="s">
-        <v>5</v>
+      <c r="AK13" s="4"/>
+    </row>
+    <row r="14" ht="15" customHeight="1">
+      <c r="A14" s="5"/>
+      <c r="B14" t="s" s="13">
+        <v>4</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -1121,9 +2085,10 @@
       <c r="AH14" s="6"/>
       <c r="AI14" s="6"/>
       <c r="AJ14" s="6"/>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
+      <c r="AK14" s="4"/>
+    </row>
+    <row r="15" ht="15" customHeight="1">
+      <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -1159,11 +2124,12 @@
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
       <c r="AJ15" s="6"/>
-    </row>
-    <row r="16" spans="1:37" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="9" t="s">
-        <v>3</v>
+      <c r="AK15" s="4"/>
+    </row>
+    <row r="16" ht="18" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" t="s" s="10">
+        <v>5</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1199,9 +2165,10 @@
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
       <c r="AJ16" s="6"/>
-    </row>
-    <row r="17" spans="1:36" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
+      <c r="AK16" s="4"/>
+    </row>
+    <row r="17" ht="8" customHeight="1">
+      <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -1237,11 +2204,12 @@
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
       <c r="AJ17" s="6"/>
-    </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7" t="s">
-        <v>11</v>
+      <c r="AK17" s="4"/>
+    </row>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" t="s" s="13">
+        <v>6</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -1277,9 +2245,10 @@
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
       <c r="AJ18" s="6"/>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="AK18" s="4"/>
+    </row>
+    <row r="19" ht="15" customHeight="1">
+      <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -1315,9 +2284,10 @@
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
       <c r="AJ19" s="6"/>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="AK19" s="4"/>
+    </row>
+    <row r="20" ht="15" customHeight="1">
+      <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -1353,9 +2323,10 @@
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
       <c r="AJ20" s="6"/>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+      <c r="AK20" s="4"/>
+    </row>
+    <row r="21" ht="15" customHeight="1">
+      <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -1391,9 +2362,10 @@
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
       <c r="AJ21" s="6"/>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+      <c r="AK21" s="4"/>
+    </row>
+    <row r="22" ht="15" customHeight="1">
+      <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1429,9 +2401,10 @@
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
       <c r="AJ22" s="6"/>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="AK22" s="4"/>
+    </row>
+    <row r="23" ht="15" customHeight="1">
+      <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -1467,9 +2440,10 @@
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
       <c r="AJ23" s="6"/>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+      <c r="AK23" s="4"/>
+    </row>
+    <row r="24" ht="15" customHeight="1">
+      <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1505,9 +2479,10 @@
       <c r="AH24" s="6"/>
       <c r="AI24" s="6"/>
       <c r="AJ24" s="6"/>
-    </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
+      <c r="AK24" s="4"/>
+    </row>
+    <row r="25" ht="15" customHeight="1">
+      <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -1543,9 +2518,10 @@
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
       <c r="AJ25" s="6"/>
-    </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+      <c r="AK25" s="4"/>
+    </row>
+    <row r="26" ht="15" customHeight="1">
+      <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -1581,9 +2557,10 @@
       <c r="AH26" s="6"/>
       <c r="AI26" s="6"/>
       <c r="AJ26" s="6"/>
-    </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
+      <c r="AK26" s="4"/>
+    </row>
+    <row r="27" ht="15" customHeight="1">
+      <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -1619,9 +2596,10 @@
       <c r="AH27" s="6"/>
       <c r="AI27" s="6"/>
       <c r="AJ27" s="6"/>
-    </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+      <c r="AK27" s="4"/>
+    </row>
+    <row r="28" ht="15" customHeight="1">
+      <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -1657,9 +2635,10 @@
       <c r="AH28" s="6"/>
       <c r="AI28" s="6"/>
       <c r="AJ28" s="6"/>
-    </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
+      <c r="AK28" s="4"/>
+    </row>
+    <row r="29" ht="15" customHeight="1">
+      <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -1695,9 +2674,10 @@
       <c r="AH29" s="6"/>
       <c r="AI29" s="6"/>
       <c r="AJ29" s="6"/>
-    </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
+      <c r="AK29" s="4"/>
+    </row>
+    <row r="30" ht="15" customHeight="1">
+      <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -1733,9 +2713,10 @@
       <c r="AH30" s="6"/>
       <c r="AI30" s="6"/>
       <c r="AJ30" s="6"/>
-    </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
+      <c r="AK30" s="4"/>
+    </row>
+    <row r="31" ht="15" customHeight="1">
+      <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -1771,9 +2752,10 @@
       <c r="AH31" s="6"/>
       <c r="AI31" s="6"/>
       <c r="AJ31" s="6"/>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+      <c r="AK31" s="4"/>
+    </row>
+    <row r="32" ht="15" customHeight="1">
+      <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -1809,9 +2791,10 @@
       <c r="AH32" s="6"/>
       <c r="AI32" s="6"/>
       <c r="AJ32" s="6"/>
-    </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
+      <c r="AK32" s="4"/>
+    </row>
+    <row r="33" ht="15" customHeight="1">
+      <c r="A33" s="5"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -1847,9 +2830,10 @@
       <c r="AH33" s="6"/>
       <c r="AI33" s="6"/>
       <c r="AJ33" s="6"/>
-    </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
+      <c r="AK33" s="4"/>
+    </row>
+    <row r="34" ht="15" customHeight="1">
+      <c r="A34" s="5"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -1885,9 +2869,10 @@
       <c r="AH34" s="6"/>
       <c r="AI34" s="6"/>
       <c r="AJ34" s="6"/>
-    </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
+      <c r="AK34" s="4"/>
+    </row>
+    <row r="35" ht="15" customHeight="1">
+      <c r="A35" s="5"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -1923,9 +2908,10 @@
       <c r="AH35" s="6"/>
       <c r="AI35" s="6"/>
       <c r="AJ35" s="6"/>
-    </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
+      <c r="AK35" s="4"/>
+    </row>
+    <row r="36" ht="15" customHeight="1">
+      <c r="A36" s="5"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -1961,9 +2947,10 @@
       <c r="AH36" s="6"/>
       <c r="AI36" s="6"/>
       <c r="AJ36" s="6"/>
-    </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
+      <c r="AK36" s="4"/>
+    </row>
+    <row r="37" ht="15" customHeight="1">
+      <c r="A37" s="5"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -1999,9 +2986,10 @@
       <c r="AH37" s="6"/>
       <c r="AI37" s="6"/>
       <c r="AJ37" s="6"/>
-    </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
+      <c r="AK37" s="4"/>
+    </row>
+    <row r="38" ht="15" customHeight="1">
+      <c r="A38" s="5"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
@@ -2037,9 +3025,10 @@
       <c r="AH38" s="6"/>
       <c r="AI38" s="6"/>
       <c r="AJ38" s="6"/>
-    </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
+      <c r="AK38" s="4"/>
+    </row>
+    <row r="39" ht="15" customHeight="1">
+      <c r="A39" s="5"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -2075,9 +3064,10 @@
       <c r="AH39" s="6"/>
       <c r="AI39" s="6"/>
       <c r="AJ39" s="6"/>
-    </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
+      <c r="AK39" s="4"/>
+    </row>
+    <row r="40" ht="15" customHeight="1">
+      <c r="A40" s="5"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -2113,9 +3103,10 @@
       <c r="AH40" s="6"/>
       <c r="AI40" s="6"/>
       <c r="AJ40" s="6"/>
-    </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
+      <c r="AK40" s="4"/>
+    </row>
+    <row r="41" ht="15" customHeight="1">
+      <c r="A41" s="5"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -2151,9 +3142,10 @@
       <c r="AH41" s="6"/>
       <c r="AI41" s="6"/>
       <c r="AJ41" s="6"/>
-    </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
+      <c r="AK41" s="4"/>
+    </row>
+    <row r="42" ht="15" customHeight="1">
+      <c r="A42" s="5"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -2189,9 +3181,10 @@
       <c r="AH42" s="6"/>
       <c r="AI42" s="6"/>
       <c r="AJ42" s="6"/>
-    </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
+      <c r="AK42" s="4"/>
+    </row>
+    <row r="43" ht="15" customHeight="1">
+      <c r="A43" s="5"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -2227,9 +3220,10 @@
       <c r="AH43" s="6"/>
       <c r="AI43" s="6"/>
       <c r="AJ43" s="6"/>
-    </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
+      <c r="AK43" s="4"/>
+    </row>
+    <row r="44" ht="15" customHeight="1">
+      <c r="A44" s="5"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -2265,9 +3259,10 @@
       <c r="AH44" s="6"/>
       <c r="AI44" s="6"/>
       <c r="AJ44" s="6"/>
-    </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
+      <c r="AK44" s="4"/>
+    </row>
+    <row r="45" ht="15" customHeight="1">
+      <c r="A45" s="5"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
@@ -2303,9 +3298,10 @@
       <c r="AH45" s="6"/>
       <c r="AI45" s="6"/>
       <c r="AJ45" s="6"/>
-    </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
+      <c r="AK45" s="4"/>
+    </row>
+    <row r="46" ht="15" customHeight="1">
+      <c r="A46" s="5"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
@@ -2341,9 +3337,10 @@
       <c r="AH46" s="6"/>
       <c r="AI46" s="6"/>
       <c r="AJ46" s="6"/>
-    </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
+      <c r="AK46" s="4"/>
+    </row>
+    <row r="47" ht="15" customHeight="1">
+      <c r="A47" s="5"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -2379,9 +3376,10 @@
       <c r="AH47" s="6"/>
       <c r="AI47" s="6"/>
       <c r="AJ47" s="6"/>
-    </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
+      <c r="AK47" s="4"/>
+    </row>
+    <row r="48" ht="15" customHeight="1">
+      <c r="A48" s="5"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
@@ -2417,9 +3415,10 @@
       <c r="AH48" s="6"/>
       <c r="AI48" s="6"/>
       <c r="AJ48" s="6"/>
-    </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
+      <c r="AK48" s="4"/>
+    </row>
+    <row r="49" ht="15" customHeight="1">
+      <c r="A49" s="5"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
@@ -2455,9 +3454,10 @@
       <c r="AH49" s="6"/>
       <c r="AI49" s="6"/>
       <c r="AJ49" s="6"/>
-    </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
+      <c r="AK49" s="4"/>
+    </row>
+    <row r="50" ht="15" customHeight="1">
+      <c r="A50" s="5"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
@@ -2493,156 +3493,198 @@
       <c r="AH50" s="6"/>
       <c r="AI50" s="6"/>
       <c r="AJ50" s="6"/>
-    </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-      <c r="P51" s="6"/>
-      <c r="Q51" s="6"/>
-      <c r="R51" s="6"/>
-      <c r="S51" s="6"/>
-      <c r="T51" s="6"/>
-      <c r="U51" s="6"/>
-      <c r="V51" s="6"/>
-      <c r="W51" s="6"/>
-      <c r="X51" s="6"/>
-      <c r="Y51" s="6"/>
-      <c r="Z51" s="6"/>
-      <c r="AA51" s="6"/>
-      <c r="AB51" s="6"/>
-      <c r="AC51" s="6"/>
-      <c r="AD51" s="6"/>
-      <c r="AE51" s="6"/>
-      <c r="AF51" s="6"/>
-      <c r="AG51" s="6"/>
-      <c r="AH51" s="6"/>
-      <c r="AI51" s="6"/>
-      <c r="AJ51" s="6"/>
+      <c r="AK50" s="4"/>
+    </row>
+    <row r="51" ht="15" customHeight="1">
+      <c r="A51" s="14"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
+      <c r="Q51" s="15"/>
+      <c r="R51" s="15"/>
+      <c r="S51" s="15"/>
+      <c r="T51" s="15"/>
+      <c r="U51" s="15"/>
+      <c r="V51" s="15"/>
+      <c r="W51" s="15"/>
+      <c r="X51" s="15"/>
+      <c r="Y51" s="15"/>
+      <c r="Z51" s="15"/>
+      <c r="AA51" s="15"/>
+      <c r="AB51" s="15"/>
+      <c r="AC51" s="15"/>
+      <c r="AD51" s="15"/>
+      <c r="AE51" s="15"/>
+      <c r="AF51" s="15"/>
+      <c r="AG51" s="15"/>
+      <c r="AH51" s="15"/>
+      <c r="AI51" s="15"/>
+      <c r="AJ51" s="15"/>
+      <c r="AK51" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="53" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="1" max="1" width="21.1719" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.6719" style="16" customWidth="1"/>
+    <col min="3" max="3" width="21.6719" style="16" customWidth="1"/>
+    <col min="4" max="4" width="20" style="16" customWidth="1"/>
+    <col min="5" max="5" width="21" style="16" customWidth="1"/>
+    <col min="6" max="256" width="8.85156" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" ht="39" customHeight="1">
+      <c r="A1" t="s" s="17">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
+      <c r="B1" t="s" s="18">
+        <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" t="s" s="18">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s" s="18">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="19">
+        <v>43101</v>
+      </c>
+      <c r="B2" s="20">
+        <v>43281</v>
+      </c>
+      <c r="C2" t="s" s="21">
+        <v>12</v>
+      </c>
+      <c r="D2" s="22">
+        <v>123</v>
+      </c>
+      <c r="E2" s="22">
+        <v>123456.78</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="19">
+        <v>43101</v>
+      </c>
+      <c r="B3" s="20">
+        <v>43281</v>
+      </c>
+      <c r="C3" t="s" s="21">
+        <v>13</v>
+      </c>
+      <c r="D3" s="22">
+        <v>1234</v>
+      </c>
+      <c r="E3" s="22">
+        <v>23456.78</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="19">
+        <v>43101</v>
+      </c>
+      <c r="B4" s="20">
+        <v>43281</v>
+      </c>
+      <c r="C4" t="s" s="21">
+        <v>14</v>
+      </c>
+      <c r="D4" s="22">
+        <v>12</v>
+      </c>
+      <c r="E4" s="22">
+        <v>3456.78</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="19">
+        <v>43101</v>
+      </c>
+      <c r="B5" s="20">
+        <v>43281</v>
+      </c>
+      <c r="C5" t="s" s="21">
+        <v>15</v>
+      </c>
+      <c r="D5" s="22">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>43101</v>
-      </c>
-      <c r="B2" s="2">
-        <v>43281</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="4">
-        <v>123</v>
-      </c>
-      <c r="E2" s="4">
-        <v>123456.78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>43101</v>
-      </c>
-      <c r="B3" s="2">
-        <v>43281</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1234</v>
-      </c>
-      <c r="E3" s="4">
-        <v>23456.78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>43101</v>
-      </c>
-      <c r="B4" s="2">
-        <v>43281</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4">
-        <v>12</v>
-      </c>
-      <c r="E4" s="4">
-        <v>3456.78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>43101</v>
-      </c>
-      <c r="B5" s="2">
-        <v>43281</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="E5" s="22">
         <v>456.78</v>
       </c>
     </row>
+    <row r="6" ht="16.5" customHeight="1">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" ht="16" customHeight="1">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+    </row>
+    <row r="8" ht="16" customHeight="1">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+    </row>
+    <row r="9" ht="16" customHeight="1">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+    </row>
+    <row r="10" ht="16" customHeight="1">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>